<commit_message>
added harvard case classification
</commit_message>
<xml_diff>
--- a/individual_results/avey/104.xlsx
+++ b/individual_results/avey/104.xlsx
@@ -564,7 +564,7 @@
         <v>0.4</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -585,7 +585,7 @@
         <v>0.5</v>
       </c>
       <c r="M2" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="N2" t="n">
         <v>0.6</v>
@@ -597,7 +597,7 @@
         <v>0.375</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="R2" t="n">
         <v>0.3333333333333333</v>
@@ -615,7 +615,7 @@
         <v>1</v>
       </c>
       <c r="W2" t="n">
-        <v>0.6666666666666666</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -637,7 +637,7 @@
         <v>0.4</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -658,7 +658,7 @@
         <v>0.2</v>
       </c>
       <c r="M3" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="N3" t="n">
         <v>0.6</v>
@@ -670,7 +670,7 @@
         <v>0.6</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="R3" t="n">
         <v>0.2</v>
@@ -688,7 +688,7 @@
         <v>0.6</v>
       </c>
       <c r="W3" t="n">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="4">
@@ -709,7 +709,9 @@
       <c r="E4" t="n">
         <v>0.4000000000000001</v>
       </c>
-      <c r="F4" t="inlineStr"/>
+      <c r="F4" t="n">
+        <v>0.1818181818181818</v>
+      </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="n">
         <v>0.3333333333333334</v>
@@ -725,7 +727,7 @@
         <v>0.2857142857142858</v>
       </c>
       <c r="M4" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="N4" t="n">
         <v>0.6</v>
@@ -737,7 +739,7 @@
         <v>0.4615384615384615</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.1818181818181818</v>
+        <v>0.3636363636363636</v>
       </c>
       <c r="R4" t="n">
         <v>0.25</v>
@@ -755,7 +757,7 @@
         <v>0.7499999999999999</v>
       </c>
       <c r="W4" t="n">
-        <v>0.5</v>
+        <v>0.7499999999999999</v>
       </c>
     </row>
     <row r="5">
@@ -776,7 +778,9 @@
       <c r="E5" t="n">
         <v>0.4</v>
       </c>
-      <c r="F5" t="inlineStr"/>
+      <c r="F5" t="n">
+        <v>0.1923076923076923</v>
+      </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="n">
         <v>0.2380952380952381</v>
@@ -792,7 +796,7 @@
         <v>0.2272727272727273</v>
       </c>
       <c r="M5" t="n">
-        <v>0.2173913043478261</v>
+        <v>0.4347826086956522</v>
       </c>
       <c r="N5" t="n">
         <v>0.6</v>
@@ -804,7 +808,7 @@
         <v>0.5357142857142857</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.1923076923076923</v>
+        <v>0.3846153846153846</v>
       </c>
       <c r="R5" t="n">
         <v>0.2173913043478261</v>
@@ -822,7 +826,7 @@
         <v>0.6521739130434783</v>
       </c>
       <c r="W5" t="n">
-        <v>0.4347826086956522</v>
+        <v>0.6521739130434783</v>
       </c>
     </row>
     <row r="6">
@@ -844,7 +848,7 @@
         <v>0.230369943897149</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>0.06572774036705124</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -865,7 +869,7 @@
         <v>0.6791866504595295</v>
       </c>
       <c r="M6" t="n">
-        <v>0.6791866504595295</v>
+        <v>0.7120505206430552</v>
       </c>
       <c r="N6" t="n">
         <v>0.4810478209239648</v>
@@ -877,7 +881,7 @@
         <v>0.4067518814962173</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.07668236376155978</v>
+        <v>0.142410104128611</v>
       </c>
       <c r="R6" t="n">
         <v>0.3395933252297648</v>
@@ -895,7 +899,7 @@
         <v>0.7973386012536817</v>
       </c>
       <c r="W6" t="n">
-        <v>0.7558690142210893</v>
+        <v>0.7973386012536817</v>
       </c>
     </row>
     <row r="7">

</xml_diff>